<commit_message>
all files are modified
</commit_message>
<xml_diff>
--- a/src/main/java/testData/TFios.xlsx
+++ b/src/main/java/testData/TFios.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="25831"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="26026"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\manis\selenium\exlProject\src\main\java\testData\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{D2FA0A54-E607-448C-91BB-3CE4F55C71E9}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{A2618D7A-F387-4DF8-AB47-4F0ED1CD8B1C}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-110" yWindow="-110" windowWidth="25820" windowHeight="15620" activeTab="1" xr2:uid="{F1A49775-88C7-4FD6-8A0E-F64AB35992D8}"/>
+    <workbookView xWindow="1440" yWindow="1440" windowWidth="19200" windowHeight="11260" activeTab="1" xr2:uid="{F1A49775-88C7-4FD6-8A0E-F64AB35992D8}"/>
   </bookViews>
   <sheets>
     <sheet name="logIninfo" sheetId="1" r:id="rId1"/>
@@ -83,9 +83,6 @@
     <t>Zip</t>
   </si>
   <si>
-    <t>Excel Project</t>
-  </si>
-  <si>
     <t>Techfios</t>
   </si>
   <si>
@@ -114,6 +111,9 @@
   </si>
   <si>
     <t>o023456</t>
+  </si>
+  <si>
+    <t>Prakash Mijar</t>
   </si>
 </sst>
 </file>
@@ -534,7 +534,7 @@
   <dimension ref="A1:J2"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="D8" sqref="D8"/>
+      <selection activeCell="A2" sqref="A2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
@@ -580,39 +580,39 @@
         <v>14</v>
       </c>
       <c r="J1" s="2" t="s">
-        <v>22</v>
+        <v>21</v>
       </c>
     </row>
     <row r="2" spans="1:10" x14ac:dyDescent="0.35">
       <c r="A2" t="s">
+        <v>25</v>
+      </c>
+      <c r="B2" t="s">
         <v>15</v>
       </c>
-      <c r="B2" t="s">
+      <c r="C2" s="3" t="s">
         <v>16</v>
       </c>
-      <c r="C2" s="3" t="s">
+      <c r="D2" t="s">
+        <v>24</v>
+      </c>
+      <c r="E2" t="s">
         <v>17</v>
       </c>
-      <c r="D2" t="s">
-        <v>25</v>
-      </c>
-      <c r="E2" t="s">
+      <c r="F2" t="s">
         <v>18</v>
       </c>
-      <c r="F2" t="s">
+      <c r="G2" t="s">
         <v>19</v>
       </c>
-      <c r="G2" t="s">
+      <c r="H2" t="s">
         <v>20</v>
       </c>
-      <c r="H2" t="s">
-        <v>21</v>
-      </c>
       <c r="I2" t="s">
-        <v>24</v>
+        <v>23</v>
       </c>
       <c r="J2" t="s">
-        <v>23</v>
+        <v>22</v>
       </c>
     </row>
   </sheetData>

</xml_diff>